<commit_message>
get np.array data through fun:get_data
</commit_message>
<xml_diff>
--- a/雷达物位传感器.xlsx
+++ b/雷达物位传感器.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22488" windowHeight="9372"/>
+    <workbookView windowWidth="22488" windowHeight="10331"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="104">
+  <si>
+    <t>是否必填</t>
+  </si>
+  <si>
+    <t>是否组合</t>
+  </si>
   <si>
     <t>序号</t>
   </si>
@@ -334,7 +340,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,13 +376,6 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -472,8 +471,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -486,9 +486,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -509,6 +508,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -521,30 +544,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -557,48 +556,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -617,6 +616,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -629,7 +664,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,48 +683,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,148 +798,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1296,15 +1295,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="M14" sqref="A1:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
+    <col min="1" max="1" width="9.66666666666667" customWidth="1"/>
     <col min="2" max="2" width="16.4444444444444" customWidth="1"/>
     <col min="3" max="3" width="7.66666666666667" customWidth="1"/>
     <col min="4" max="4" width="9.66666666666667" customWidth="1"/>
@@ -1324,7 +1323,10 @@
     <col min="19" max="19" width="5.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:19">
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="F1">
         <v>1</v>
       </c>
@@ -1335,10 +1337,10 @@
         <v>1</v>
       </c>
       <c r="I1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K1">
         <v>1</v>
@@ -1356,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="P1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q1">
         <v>0</v>
@@ -1365,977 +1367,1024 @@
         <v>0</v>
       </c>
       <c r="S1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" t="s">
-        <v>18</v>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="S3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="S4" t="s">
         <v>38</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>39</v>
       </c>
       <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" t="s">
         <v>38</v>
-      </c>
-      <c r="L6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" t="s">
         <v>38</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" t="s">
         <v>47</v>
       </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O8" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" t="s">
+        <v>37</v>
+      </c>
+      <c r="S8" t="s">
         <v>48</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R8" t="s">
-        <v>35</v>
-      </c>
-      <c r="S8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
         <v>49</v>
       </c>
-      <c r="D9">
-        <v>5402</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" t="s">
-        <v>55</v>
-      </c>
-      <c r="O9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" t="s">
-        <v>33</v>
+      <c r="Q9" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" t="s">
+        <v>37</v>
       </c>
       <c r="S9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>5402</v>
       </c>
       <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s">
         <v>56</v>
       </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" t="s">
         <v>57</v>
       </c>
-      <c r="L10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" t="s">
-        <v>55</v>
-      </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11">
+        <v>5402</v>
+      </c>
+      <c r="E11" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K11" t="s">
-        <v>28</v>
-      </c>
       <c r="L11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N11" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="O11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P11" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>66</v>
-      </c>
-      <c r="R11" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="S11" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>68</v>
+      </c>
+      <c r="R12" t="s">
         <v>69</v>
       </c>
-      <c r="F12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" t="s">
-        <v>64</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="S12" t="s">
         <v>70</v>
-      </c>
-      <c r="L12" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" t="s">
-        <v>32</v>
-      </c>
-      <c r="P12" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>71</v>
-      </c>
-      <c r="R12" t="s">
-        <v>67</v>
-      </c>
-      <c r="S12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" t="s">
         <v>72</v>
       </c>
-      <c r="F13" t="s">
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" t="s">
         <v>73</v>
       </c>
-      <c r="G13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K13" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" t="s">
-        <v>31</v>
-      </c>
-      <c r="O13" t="s">
-        <v>32</v>
-      </c>
-      <c r="P13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>74</v>
-      </c>
       <c r="R13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
         <v>75</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="L14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q14" t="s">
         <v>76</v>
       </c>
       <c r="R14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
         <v>77</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P15" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q15" t="s">
         <v>78</v>
       </c>
-      <c r="F15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" t="s">
-        <v>81</v>
-      </c>
-      <c r="N15" t="s">
-        <v>82</v>
-      </c>
-      <c r="O15" t="s">
-        <v>32</v>
-      </c>
-      <c r="P15" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>83</v>
+      <c r="R15" t="s">
+        <v>69</v>
       </c>
       <c r="S15" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" t="s">
+        <v>83</v>
+      </c>
+      <c r="N16" t="s">
+        <v>84</v>
+      </c>
+      <c r="O16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" t="s">
         <v>85</v>
       </c>
-      <c r="F16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" t="s">
-        <v>80</v>
-      </c>
-      <c r="L16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" t="s">
-        <v>81</v>
-      </c>
-      <c r="N16" t="s">
-        <v>82</v>
-      </c>
-      <c r="O16" t="s">
-        <v>32</v>
-      </c>
-      <c r="P16" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>86</v>
-      </c>
-      <c r="R16" t="s">
-        <v>87</v>
-      </c>
-      <c r="S16" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" t="s">
+        <v>82</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" t="s">
+        <v>83</v>
+      </c>
+      <c r="N17" t="s">
+        <v>84</v>
+      </c>
+      <c r="O17" t="s">
+        <v>34</v>
+      </c>
+      <c r="P17" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q17" t="s">
         <v>88</v>
       </c>
-      <c r="D17" t="s">
+      <c r="R17" t="s">
         <v>89</v>
       </c>
-      <c r="E17" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" t="s">
-        <v>93</v>
-      </c>
-      <c r="J17" t="s">
-        <v>94</v>
-      </c>
-      <c r="K17" t="s">
-        <v>95</v>
-      </c>
-      <c r="L17" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" t="s">
-        <v>30</v>
-      </c>
-      <c r="N17" t="s">
-        <v>96</v>
-      </c>
-      <c r="O17" t="s">
-        <v>32</v>
-      </c>
-      <c r="P17" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>98</v>
-      </c>
-      <c r="R17" t="s">
-        <v>99</v>
-      </c>
       <c r="S17" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s">
+        <v>98</v>
+      </c>
+      <c r="O18" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>100</v>
+      </c>
+      <c r="R18" t="s">
+        <v>101</v>
+      </c>
+      <c r="S18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
         <v>91</v>
       </c>
-      <c r="G18" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
         <v>93</v>
       </c>
-      <c r="J18" t="s">
+      <c r="G19" t="s">
         <v>94</v>
       </c>
-      <c r="K18" t="s">
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" t="s">
         <v>95</v>
       </c>
-      <c r="L18" t="s">
-        <v>29</v>
-      </c>
-      <c r="M18" t="s">
-        <v>30</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="J19" t="s">
         <v>96</v>
       </c>
-      <c r="O18" t="s">
+      <c r="K19" t="s">
+        <v>97</v>
+      </c>
+      <c r="L19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" t="s">
         <v>32</v>
       </c>
-      <c r="P18" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q18" t="s">
+      <c r="N19" t="s">
+        <v>98</v>
+      </c>
+      <c r="O19" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>103</v>
+      </c>
+      <c r="R19" t="s">
         <v>101</v>
       </c>
-      <c r="R18" t="s">
-        <v>99</v>
-      </c>
-      <c r="S18" t="s">
-        <v>68</v>
+      <c r="S19" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>